<commit_message>
making the excel file colorful
</commit_message>
<xml_diff>
--- a/3-WR-Major-and-trace-elements.xlsx
+++ b/3-WR-Major-and-trace-elements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aebrahimifard\Documents\TU Library\Learning\s1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aebrahimifard\Documents\TU Library\Learning\s2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -285,7 +285,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +297,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -340,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -348,6 +355,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1047,10 +1057,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C5" t="s">
@@ -1076,7 +1086,7 @@
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C6" t="s">
@@ -1102,7 +1112,7 @@
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C7" t="s">
@@ -1221,7 +1231,7 @@
       <c r="A8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C8" t="s">
@@ -1340,7 +1350,7 @@
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C9" t="s">
@@ -1459,7 +1469,7 @@
       <c r="A10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C10" t="s">
@@ -1578,7 +1588,7 @@
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C11" t="s">
@@ -1697,7 +1707,7 @@
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C12" t="s">
@@ -1816,7 +1826,7 @@
       <c r="A13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C13" t="s">
@@ -1935,7 +1945,7 @@
       <c r="A14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C14" t="s">
@@ -2054,7 +2064,7 @@
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C15" t="s">
@@ -2173,7 +2183,7 @@
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C16" t="s">
@@ -2292,7 +2302,7 @@
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C17" t="s">
@@ -2411,7 +2421,7 @@
       <c r="A18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C18" t="s">
@@ -2528,5 +2538,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
making some cells yellow
</commit_message>
<xml_diff>
--- a/3-WR-Major-and-trace-elements.xlsx
+++ b/3-WR-Major-and-trace-elements.xlsx
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -356,6 +356,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,7 +662,7 @@
   <dimension ref="A1:AR18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B18"/>
+      <selection activeCell="K10" sqref="K10:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1481,16 +1482,16 @@
       <c r="J10">
         <v>0.79</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="4">
         <v>15.4</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="4">
         <v>5.59</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
         <v>0.09</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>6.32</v>
       </c>
       <c r="O10">
@@ -1600,16 +1601,16 @@
       <c r="J11">
         <v>0.76</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>15.18</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="4">
         <v>5.0199999999999996</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <v>0.08</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="4">
         <v>5.27</v>
       </c>
       <c r="O11">
@@ -1719,16 +1720,16 @@
       <c r="J12">
         <v>0.54</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="4">
         <v>17.68</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="4">
         <v>3.61</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="4">
         <v>0.06</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="4">
         <v>1.61</v>
       </c>
       <c r="O12">
@@ -1838,16 +1839,16 @@
       <c r="J13">
         <v>0.67</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <v>17.55</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="4">
         <v>4.41</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="4">
         <v>2.02</v>
       </c>
       <c r="O13">
@@ -1957,16 +1958,16 @@
       <c r="J14">
         <v>0.81</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="4">
         <v>20.67</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="4">
         <v>5.39</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>2.4300000000000002</v>
       </c>
       <c r="O14">
@@ -2076,16 +2077,16 @@
       <c r="J15">
         <v>0.8</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <v>19.68</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="4">
         <v>5.410000000000001</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="4">
         <v>2.5499999999999998</v>
       </c>
       <c r="O15">
@@ -2195,16 +2196,16 @@
       <c r="J16">
         <v>0.74</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="4">
         <v>19.399999999999999</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="4">
         <v>5.0100000000000007</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="4">
         <v>2.2799999999999998</v>
       </c>
       <c r="O16">

</xml_diff>

<commit_message>
making some of the excell cell to yellow
</commit_message>
<xml_diff>
--- a/3-WR-Major-and-trace-elements.xlsx
+++ b/3-WR-Major-and-trace-elements.xlsx
@@ -347,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -356,6 +356,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR18"/>
+  <dimension ref="A1:AR19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B18"/>
+      <selection activeCell="H11" sqref="H11:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1594,19 +1595,20 @@
       <c r="C11" t="s">
         <v>63</v>
       </c>
-      <c r="I11">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4">
         <v>60.83</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>0.76</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <v>15.18</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="4">
         <v>5.0199999999999996</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <v>0.08</v>
       </c>
       <c r="N11">
@@ -1713,19 +1715,20 @@
       <c r="C12" t="s">
         <v>63</v>
       </c>
-      <c r="I12">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4">
         <v>64.61</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="4">
         <v>0.54</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="4">
         <v>17.68</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="4">
         <v>3.61</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="4">
         <v>0.06</v>
       </c>
       <c r="N12">
@@ -1832,19 +1835,20 @@
       <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="I13">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4">
         <v>65.03</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>0.67</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <v>17.55</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="4">
         <v>4.41</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N13">
@@ -1951,19 +1955,20 @@
       <c r="C14" t="s">
         <v>63</v>
       </c>
-      <c r="I14">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4">
         <v>60.2</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="4">
         <v>0.81</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="4">
         <v>20.67</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="4">
         <v>5.39</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N14">
@@ -2070,19 +2075,20 @@
       <c r="C15" t="s">
         <v>63</v>
       </c>
-      <c r="I15">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4">
         <v>59.97</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="4">
         <v>0.8</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <v>19.68</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="4">
         <v>5.410000000000001</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N15">
@@ -2189,19 +2195,20 @@
       <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="I16">
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
         <v>61.92</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <v>0.74</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="4">
         <v>19.399999999999999</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="4">
         <v>5.0100000000000007</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N16">
@@ -2308,19 +2315,20 @@
       <c r="C17" t="s">
         <v>63</v>
       </c>
-      <c r="I17">
+      <c r="H17" s="4"/>
+      <c r="I17" s="4">
         <v>64.760000000000005</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <v>0.59</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="4">
         <v>16.89</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="4">
         <v>4.13</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="4">
         <v>0.08</v>
       </c>
       <c r="N17">
@@ -2427,19 +2435,20 @@
       <c r="C18" t="s">
         <v>63</v>
       </c>
-      <c r="I18">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4">
         <v>65.09</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="4">
         <v>16.77</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="4">
         <v>4.1500000000000004</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="4">
         <v>0.08</v>
       </c>
       <c r="N18">
@@ -2535,6 +2544,14 @@
       <c r="AR18">
         <v>2.7972972972972969</v>
       </c>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>